<commit_message>
added cypress test scenarios
</commit_message>
<xml_diff>
--- a/test-scenarios/test_scenarios_table.xlsx
+++ b/test-scenarios/test_scenarios_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/araddavid/Documents/GitHub/Arad-Israel-semA-CV/test-scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3503008A-0CC2-334A-8126-4B572C4FDA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00574409-33E6-584F-B2A8-C5618FC5C583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="24820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
   <si>
     <t>תוצאה צפויה</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>4.3</t>
+  </si>
+  <si>
+    <t>הודעת ״התחברות מוצלחת״ ומעבר אל מסך תצוגת קורות החיים</t>
   </si>
 </sst>
 </file>
@@ -832,7 +835,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -866,7 +869,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.15">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>

</xml_diff>